<commit_message>
Revisión de Código 4
</commit_message>
<xml_diff>
--- a/Avance/Data_Ejemplo.xlsx
+++ b/Avance/Data_Ejemplo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stef\Desktop\Proyectos\ZIEMAX\Cesar Ziemax\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stef\Desktop\Proyectos\ZIEMAX\Proyecto Ziemax 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -35,7 +35,7 @@
     <author>Stef</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="77">
   <si>
     <t>Tipo servicio</t>
   </si>
@@ -253,6 +253,48 @@
   </si>
   <si>
     <t>Jerarquia de Servicio**</t>
+  </si>
+  <si>
+    <t>LimiteCantidad</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>Junior</t>
+  </si>
+  <si>
+    <t>Profesor</t>
+  </si>
+  <si>
+    <t>Experto</t>
+  </si>
+  <si>
+    <t>Informatico</t>
+  </si>
+  <si>
+    <t>Expertise2</t>
+  </si>
+  <si>
+    <t>Costo_ZIEMAX</t>
+  </si>
+  <si>
+    <t>Sueldo</t>
+  </si>
+  <si>
+    <t>Costo_Ziemax_Horas_Informatica</t>
+  </si>
+  <si>
+    <t>Costo_Ziemax_Horas_Profesor</t>
+  </si>
+  <si>
+    <t>ExperticeInfor</t>
+  </si>
+  <si>
+    <t>COSTO_HORA</t>
+  </si>
+  <si>
+    <t>COSTO_EXP_ZIEMAX</t>
   </si>
 </sst>
 </file>
@@ -957,10 +999,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L20"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,12 +1014,16 @@
     <col min="5" max="5" width="21.28515625" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
-    <col min="11" max="11" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="12" max="12" width="6.140625" customWidth="1"/>
+    <col min="14" max="14" width="31" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
@@ -1000,22 +1046,43 @@
         <v>17</v>
       </c>
       <c r="H1" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="J1" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="K1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="K1" s="9" t="s">
+      <c r="L1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="N1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1037,17 +1104,35 @@
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
       <c r="I2">
         <v>1</v>
       </c>
       <c r="J2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1070,16 +1155,37 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1102,16 +1208,37 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
         <v>3</v>
       </c>
-      <c r="J4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1134,16 +1261,37 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1166,16 +1314,37 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1198,16 +1367,37 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
         <v>3</v>
       </c>
-      <c r="J7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1230,16 +1420,37 @@
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <v>3</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>4</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>5000</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1262,16 +1473,37 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>3</v>
+      </c>
+      <c r="O9">
+        <v>2</v>
+      </c>
+      <c r="P9">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+      <c r="S9" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1294,16 +1526,37 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>3</v>
+      </c>
+      <c r="O10">
+        <v>2</v>
+      </c>
+      <c r="P10">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1326,16 +1579,37 @@
         <v>0</v>
       </c>
       <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
         <v>3</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
       <c r="J11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
+        <v>2</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+      <c r="S11" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1358,16 +1632,37 @@
         <v>0</v>
       </c>
       <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
         <v>3</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
       <c r="J12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>4</v>
+      </c>
+      <c r="O12">
+        <v>2</v>
+      </c>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+      <c r="S12" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1390,16 +1685,37 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
         <v>4</v>
       </c>
-      <c r="J13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>2</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>2</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+      <c r="S13" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1422,16 +1738,37 @@
         <v>1</v>
       </c>
       <c r="H14">
+        <v>15000</v>
+      </c>
+      <c r="I14">
         <v>3</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
       <c r="J14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>2</v>
+      </c>
+      <c r="O14">
+        <v>4</v>
+      </c>
+      <c r="P14">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+      <c r="S14" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -1454,16 +1791,37 @@
         <v>1</v>
       </c>
       <c r="H15">
+        <v>15000</v>
+      </c>
+      <c r="I15">
         <v>4</v>
       </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
       <c r="J15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <v>2</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -1486,16 +1844,37 @@
         <v>1</v>
       </c>
       <c r="H16">
+        <v>15000</v>
+      </c>
+      <c r="I16">
         <v>3</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
       <c r="J16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K16">
+        <v>1</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>4</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1518,16 +1897,37 @@
         <v>1</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>15000</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J17">
+        <v>1</v>
+      </c>
+      <c r="K17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>4</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R17">
+        <v>1</v>
+      </c>
+      <c r="S17" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>35</v>
       </c>
@@ -1550,16 +1950,37 @@
         <v>1</v>
       </c>
       <c r="H18">
-        <v>2</v>
+        <v>15000</v>
       </c>
       <c r="I18">
         <v>2</v>
       </c>
       <c r="J18">
+        <v>2</v>
+      </c>
+      <c r="K18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>4</v>
+      </c>
+      <c r="P18">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R18">
+        <v>1</v>
+      </c>
+      <c r="S18" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1582,16 +2003,37 @@
         <v>2</v>
       </c>
       <c r="H19">
+        <v>30000</v>
+      </c>
+      <c r="I19">
         <v>3</v>
       </c>
-      <c r="I19">
-        <v>2</v>
-      </c>
       <c r="J19">
+        <v>2</v>
+      </c>
+      <c r="K19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>4</v>
+      </c>
+      <c r="P19">
+        <v>2</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>6250</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19" s="5">
+        <v>5625</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1614,13 +2056,34 @@
         <v>3</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>45000</v>
       </c>
       <c r="I20">
         <v>4</v>
       </c>
       <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20">
         <v>3</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>8</v>
+      </c>
+      <c r="P20">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>9375</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20" s="5">
+        <v>5625</v>
       </c>
     </row>
   </sheetData>
@@ -1631,15 +2094,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="13.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
@@ -1649,8 +2116,17 @@
       <c r="C1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1660,8 +2136,17 @@
       <c r="C2">
         <v>15000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5000</v>
+      </c>
+      <c r="F2" s="5">
+        <v>800000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1671,8 +2156,17 @@
       <c r="C3">
         <v>30000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="5">
+        <v>6250</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1681,6 +2175,35 @@
       </c>
       <c r="C4">
         <v>45000</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="5">
+        <v>9375</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>20000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="5">
+        <v>5625</v>
+      </c>
+      <c r="F5" s="5">
+        <v>900000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>